<commit_message>
ITST-21328: xlsx-reader: Add option to skip empty rows and extend options to skip empty cells
- Extend iterator to keep track of the amount of skipped rows and their structure, thus enabling lookaheads via the reader.
- Implement new configuration option SkipEmptyRows.
- Implement new configuration "enum" ReaderSkipConfiguration for configuration of different skip behaviors.
- Adapt SkipEmptyCells to make use of ReaderSkipConfiguration as well, for consistency.
- Extend SkipEmptyCells handling with the option to skip only trailing empty cells.
- Extend tests to cover the new behavior.
- Adapt readme example code.
- Prepare changelog for release.
</commit_message>
<xml_diff>
--- a/tests/input_files/empty_rows_test.xlsx
+++ b/tests/input_files/empty_rows_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp_content\xlsx_reader\tests\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A192D21B-0A33-420D-A48C-42DA582B36E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB23BF2B-ADD4-4155-8F29-C3DDEB46A9F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="3630" windowWidth="21600" windowHeight="11505" xr2:uid="{2BEAEF28-1BED-4D7A-B537-E8507A3B578F}"/>
+    <workbookView xWindow="4275" yWindow="3675" windowWidth="21600" windowHeight="11505" xr2:uid="{2BEAEF28-1BED-4D7A-B537-E8507A3B578F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD45CD7-9A65-487C-849B-3B3CE5DDA3AE}">
-  <dimension ref="B2:B5"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,6 +429,10 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>